<commit_message>
Duplicated catalogue values for NatRel deleted
</commit_message>
<xml_diff>
--- a/scr/DM_Asset_Catalogues.xlsx
+++ b/scr/DM_Asset_Catalogues.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Appl\DATA\PROD\lg\01_PRODUKTION\Datenmodell\34-Unterstuetzung_tech_Modellierung\DM-Asset\work\dmAssets\work\catalogues\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Appl\DATA\PROD\lg\01_PRODUKTION\Datenmodell\34-Unterstuetzung_tech_Modellierung\DM-Asset\work\dmAssets\scr\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14145" tabRatio="759" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14145" tabRatio="759"/>
   </bookViews>
   <sheets>
     <sheet name="AssetKindItem" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="AutoCatLabelItem" sheetId="4" r:id="rId3"/>
     <sheet name="AutoObjectCatItem" sheetId="5" r:id="rId4"/>
     <sheet name="AssetFormatItem" sheetId="6" r:id="rId5"/>
-    <sheet name="NatRelItem" sheetId="7" r:id="rId6"/>
+    <sheet name="NatRelItem" sheetId="11" r:id="rId6"/>
     <sheet name="ContactKindItem" sheetId="8" r:id="rId7"/>
     <sheet name="PubChannelItem" sheetId="9" r:id="rId8"/>
     <sheet name="StatusWorkItem" sheetId="10" r:id="rId9"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="344">
   <si>
     <t>T_Id</t>
   </si>
@@ -812,9 +812,6 @@
     <t>geolWasteDisp</t>
   </si>
   <si>
-    <t>1b1c8960-e42b-494a-8efd-a71723e6ec39</t>
-  </si>
-  <si>
     <t>Prospektion und Föderung von Rohstoffen aus dem Energiebereich</t>
   </si>
   <si>
@@ -869,43 +866,7 @@
     <t>5cec87c4-6d6c-43e4-a358-97004c5af97b</t>
   </si>
   <si>
-    <t>87d5eb23-403e-4854-9efd-6d7347a8a472</t>
-  </si>
-  <si>
-    <t>e620a3eb-4674-4607-89ad-cfda9d8c4e58</t>
-  </si>
-  <si>
     <t>67206d59-5f89-481f-980e-d49887f9121a</t>
-  </si>
-  <si>
-    <t>Prospektion und Föderung von Rohstoffen im Energiebereich</t>
-  </si>
-  <si>
-    <t>d5250db9-7cbb-4994-b481-7e7b5bc5bfad</t>
-  </si>
-  <si>
-    <t>Resultate der SGPK</t>
-  </si>
-  <si>
-    <t>SGPK</t>
-  </si>
-  <si>
-    <t>7ce9ae76-5694-4cb7-8569-3388646a415f</t>
-  </si>
-  <si>
-    <t>SGTK_FGS</t>
-  </si>
-  <si>
-    <t>80c729d1-d644-489a-92a1-aa625fa14425</t>
-  </si>
-  <si>
-    <t>1f46125e-550f-4bc8-b726-e78f6fcdd100</t>
-  </si>
-  <si>
-    <t>41a56484-79f8-497d-b3d2-2a374a9208be</t>
-  </si>
-  <si>
-    <t>a10f4b26-0117-4dd5-a8be-d1bce547ee03</t>
   </si>
   <si>
     <t>5bf99498-3140-483a-8b3a-1510109637a2</t>
@@ -1415,7 +1376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -3358,10 +3319,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3428,108 +3389,108 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="C2" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="D2" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>74</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="C3" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D3" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D4" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="B5" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="C5" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="D5" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="C6" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="D6" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>78</v>
+        <v>126</v>
       </c>
       <c r="B7" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="C7" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D7" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>79</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>282</v>
+        <v>263</v>
       </c>
       <c r="C8" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D8" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>80</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
       <c r="C9" t="s">
         <v>257</v>
@@ -3540,141 +3501,15 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="B10" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="C10" t="s">
         <v>254</v>
       </c>
       <c r="D10" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>122</v>
-      </c>
-      <c r="B11" t="s">
-        <v>279</v>
-      </c>
-      <c r="C11" t="s">
-        <v>278</v>
-      </c>
-      <c r="D11" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>123</v>
-      </c>
-      <c r="B12" t="s">
-        <v>276</v>
-      </c>
-      <c r="C12" t="s">
-        <v>275</v>
-      </c>
-      <c r="D12" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>124</v>
-      </c>
-      <c r="B13" t="s">
-        <v>273</v>
-      </c>
-      <c r="C13" t="s">
-        <v>272</v>
-      </c>
-      <c r="D13" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>125</v>
-      </c>
-      <c r="B14" t="s">
-        <v>270</v>
-      </c>
-      <c r="C14" t="s">
-        <v>269</v>
-      </c>
-      <c r="D14" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>126</v>
-      </c>
-      <c r="B15" t="s">
-        <v>267</v>
-      </c>
-      <c r="C15" t="s">
-        <v>266</v>
-      </c>
-      <c r="D15" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>127</v>
-      </c>
-      <c r="B16" t="s">
-        <v>264</v>
-      </c>
-      <c r="C16" t="s">
-        <v>263</v>
-      </c>
-      <c r="D16" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>128</v>
-      </c>
-      <c r="B17" t="s">
-        <v>261</v>
-      </c>
-      <c r="C17" t="s">
-        <v>260</v>
-      </c>
-      <c r="D17" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>129</v>
-      </c>
-      <c r="B18" t="s">
-        <v>258</v>
-      </c>
-      <c r="C18" t="s">
-        <v>257</v>
-      </c>
-      <c r="D18" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>130</v>
-      </c>
-      <c r="B19" t="s">
-        <v>255</v>
-      </c>
-      <c r="C19" t="s">
-        <v>254</v>
-      </c>
-      <c r="D19" t="s">
         <v>253</v>
       </c>
     </row>
@@ -3758,13 +3593,13 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="C2" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="D2" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -3772,7 +3607,7 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -3786,13 +3621,13 @@
         <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="C4" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="D4" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -3800,13 +3635,13 @@
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="C5" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="D5" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -3814,13 +3649,13 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="C6" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="D6" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -3828,13 +3663,13 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="C7" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="D7" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -3842,7 +3677,7 @@
         <v>146</v>
       </c>
       <c r="B8" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="C8" t="s">
         <v>113</v>
@@ -3951,13 +3786,13 @@
         <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="C2" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="D2" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="O2" t="s">
         <v>26</v>
@@ -3971,13 +3806,13 @@
         <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="C3" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="D3" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="O3" t="s">
         <v>26</v>
@@ -3991,13 +3826,13 @@
         <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="C4" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="D4" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="O4" t="s">
         <v>26</v>
@@ -4011,13 +3846,13 @@
         <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="C5" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="D5" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="O5" t="s">
         <v>22</v>
@@ -4031,13 +3866,13 @@
         <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="C6" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="D6" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="O6" t="s">
         <v>26</v>
@@ -4046,7 +3881,7 @@
         <v>22</v>
       </c>
       <c r="R6" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
@@ -4054,16 +3889,16 @@
         <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="C7" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="D7" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="J7" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="O7" t="s">
         <v>26</v>
@@ -4072,7 +3907,7 @@
         <v>22</v>
       </c>
       <c r="R7" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -4080,13 +3915,13 @@
         <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="O8" t="s">
         <v>26</v>
@@ -4104,7 +3939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -4175,13 +4010,13 @@
         <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>356</v>
+        <v>343</v>
       </c>
       <c r="C2" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="D2" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -4189,13 +4024,13 @@
         <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="C3" t="s">
-        <v>352</v>
+        <v>339</v>
       </c>
       <c r="D3" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -4203,13 +4038,13 @@
         <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="C4" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="D4" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -4217,13 +4052,13 @@
         <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
       <c r="C5" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="D5" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -4231,13 +4066,13 @@
         <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="C6" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="D6" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -4245,13 +4080,13 @@
         <v>87</v>
       </c>
       <c r="B7" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="C7" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="D7" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -4259,13 +4094,13 @@
         <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="C8" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="D8" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -4273,13 +4108,13 @@
         <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="C9" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="D9" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -4287,13 +4122,13 @@
         <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="C10" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="D10" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>